<commit_message>
add monte_carlo and update database
</commit_message>
<xml_diff>
--- a/database/industries/bargh/bemoto/income/quarterly/dollar.xlsx
+++ b/database/industries/bargh/bemoto/income/quarterly/dollar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EBRAHIMI\Desktop\Trade\database\industries\bargh\bemoto\income\quarterly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VAHID\Desktop\Trade\database\industries\bargh\bemoto\income\quarterly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC68C845-7156-4674-A8B2-4974BBD75208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B193E79-C4CB-4C8E-82A0-D8E1479DFF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
     <t>1401-10-28 (2)</t>
   </si>
   <si>
-    <t>1402-02-23 (5)</t>
+    <t>1402-03-09 (6)</t>
   </si>
   <si>
     <t>1401-04-28</t>
@@ -94,7 +94,7 @@
     <t>1401-10-28</t>
   </si>
   <si>
-    <t>1402-02-23 (2)</t>
+    <t>1402-03-09 (3)</t>
   </si>
   <si>
     <t>فروش</t>
@@ -891,7 +891,7 @@
         <v>-12222</v>
       </c>
       <c r="M12" s="11">
-        <v>-16977</v>
+        <v>-16914</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
@@ -927,7 +927,7 @@
         <v>6114</v>
       </c>
       <c r="M13" s="15">
-        <v>8377</v>
+        <v>8439</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
@@ -963,7 +963,7 @@
         <v>-341</v>
       </c>
       <c r="M14" s="11">
-        <v>-631</v>
+        <v>-695</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
@@ -1071,7 +1071,7 @@
         <v>6144</v>
       </c>
       <c r="M17" s="15">
-        <v>8771</v>
+        <v>8769</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
@@ -1179,7 +1179,7 @@
         <v>5224</v>
       </c>
       <c r="M20" s="17">
-        <v>8269</v>
+        <v>8267</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
@@ -1215,7 +1215,7 @@
         <v>-860</v>
       </c>
       <c r="M21" s="13">
-        <v>-2242</v>
+        <v>-1788</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
@@ -1251,7 +1251,7 @@
         <v>4364</v>
       </c>
       <c r="M22" s="17">
-        <v>6027</v>
+        <v>6479</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
@@ -1323,7 +1323,7 @@
         <v>4364</v>
       </c>
       <c r="M24" s="17">
-        <v>6027</v>
+        <v>6479</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">

</xml_diff>